<commit_message>
new php file and excel file
</commit_message>
<xml_diff>
--- a/e_food.xlsx
+++ b/e_food.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="6555"/>
+    <workbookView windowWidth="20490" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -136,8 +136,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
@@ -150,12 +150,71 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -171,30 +230,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -208,67 +262,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -277,23 +270,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,19 +314,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.8"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -338,181 +470,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,11 +529,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -561,21 +555,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -597,15 +576,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -615,17 +585,35 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -643,7 +631,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -661,134 +649,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -796,18 +784,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1246,12 +1228,12 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
     <row r="4" spans="2:14">
       <c r="B4" s="1" t="s">
@@ -1266,16 +1248,16 @@
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1292,16 +1274,16 @@
       <c r="E5" s="1">
         <v>9908332221</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="4">
         <v>50</v>
       </c>
     </row>
@@ -1318,16 +1300,16 @@
       <c r="E6" s="1">
         <v>8900388312</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="4">
         <v>75</v>
       </c>
     </row>
@@ -1336,44 +1318,44 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="4">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="11:14">
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="M8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="4">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="11:14">
-      <c r="K9" s="6" t="s">
+      <c r="K9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="L9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="6" t="s">
+      <c r="M9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="4">
         <v>55</v>
       </c>
     </row>
@@ -1381,16 +1363,16 @@
       <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="K10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="M10" s="6" t="s">
+      <c r="M10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="4">
         <v>35</v>
       </c>
     </row>
@@ -1407,7 +1389,7 @@
       <c r="E12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1424,7 +1406,7 @@
       <c r="E13" s="2">
         <v>1</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>75</v>
       </c>
     </row>
@@ -1441,7 +1423,7 @@
       <c r="E14" s="2">
         <v>1</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>45</v>
       </c>
     </row>
@@ -1458,7 +1440,7 @@
       <c r="E15" s="2">
         <v>1</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <v>55</v>
       </c>
     </row>
@@ -1467,7 +1449,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>